<commit_message>
refactored in aufgabe 7
</commit_message>
<xml_diff>
--- a/Aufgabe06/Bewertung.xlsx
+++ b/Aufgabe06/Bewertung.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E69FCDF-7F66-4A3D-BF17-128F95535A27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F5666B-1615-499C-9077-426A2326F71B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="69">
   <si>
     <t>User Id</t>
   </si>
@@ -225,6 +225,12 @@
   </si>
   <si>
     <t>Is picture exercise6-4-CopyConstr02.jpg uploaded to SVN to show code of  copy-constructor of second class (different from AtcoCommand of exercise 6-3)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">siehe Feedback-Datei </t>
+  </si>
+  <si>
+    <t>siehe Feedback, könnte man geschickter machen, zu viele Ausgaben</t>
   </si>
 </sst>
 </file>
@@ -235,7 +241,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0_ ;[Red]\-0\ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,6 +258,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -307,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -355,6 +368,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -638,7 +652,7 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,7 +892,7 @@
       <c r="D16" s="7"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>28</v>
       </c>
@@ -895,50 +909,56 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C18" s="7">
         <v>3</v>
       </c>
       <c r="D18" s="15">
         <f>IF(B18="yes",C18,-5)</f>
-        <v>3</v>
+        <v>-5</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>2</v>
+      <c r="B19" s="23" t="s">
+        <v>21</v>
       </c>
       <c r="C19" s="7">
         <v>3</v>
       </c>
       <c r="D19" s="7">
         <f t="shared" ref="D19" si="0">IF(B19="yes",C19,0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>38</v>
       </c>
@@ -955,7 +975,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>3</v>
       </c>
@@ -973,14 +993,14 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>39</v>
       </c>
@@ -997,7 +1017,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>3</v>
       </c>
@@ -1015,7 +1035,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>3</v>
       </c>
@@ -1033,14 +1053,14 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>40</v>
       </c>
@@ -1057,7 +1077,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>3</v>
       </c>
@@ -1075,7 +1095,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>3</v>
       </c>
@@ -1093,7 +1113,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>3</v>
       </c>
@@ -1111,7 +1131,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>3</v>
       </c>
@@ -1129,7 +1149,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>41</v>
       </c>
@@ -1146,7 +1166,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>3</v>
       </c>
@@ -1164,7 +1184,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>3</v>
       </c>
@@ -1182,7 +1202,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>3</v>
       </c>
@@ -1200,7 +1220,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>3</v>
       </c>
@@ -1218,7 +1238,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>3</v>
       </c>
@@ -1236,7 +1256,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>3</v>
       </c>
@@ -1254,7 +1274,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>3</v>
       </c>
@@ -1272,7 +1292,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>3</v>
       </c>
@@ -1290,7 +1310,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>3</v>
       </c>
@@ -1308,7 +1328,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>3</v>
       </c>
@@ -1326,7 +1346,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
         <v>56</v>
       </c>
@@ -1335,7 +1355,7 @@
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
     </row>
-    <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>3</v>
       </c>
@@ -1355,8 +1375,11 @@
       <c r="G45" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H45" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>3</v>
       </c>
@@ -1377,14 +1400,14 @@
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -1418,7 +1441,7 @@
       <c r="C51" s="7"/>
       <c r="D51" s="7">
         <f>MAX(0,SUM(D13:D47))</f>
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E51" s="3"/>
     </row>
@@ -1440,7 +1463,7 @@
       <c r="C53" s="7"/>
       <c r="D53" s="17">
         <f>IF(B52="Bachelor",D51/(D50-8),D51/(D50))</f>
-        <v>1.2105263157894737</v>
+        <v>0.92105263157894735</v>
       </c>
       <c r="E53" s="3"/>
     </row>

</xml_diff>